<commit_message>
fix minor bug on calculate in Standard deviation for Algorithm 2 file
</commit_message>
<xml_diff>
--- a/Standard deviation for Algorithm 2.xlsx
+++ b/Standard deviation for Algorithm 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\eclipse-workspace\GeoApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvir\Documents\Ariel University\Eclipse Workspace\GeoApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -119,14 +119,14 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="חישוב" xfId="1" builtinId="22"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -406,36 +406,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="16.3984375" customWidth="1"/>
+    <col min="5" max="5" width="15.19921875" customWidth="1"/>
     <col min="13" max="13" width="16.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
       <c r="M1" t="s">
         <v>8</v>
       </c>
@@ -473,19 +475,19 @@
       </c>
       <c r="J2">
         <f>AVERAGE(G2,G4:G8,G11:G36,G38,G40,G46:G49,G54:G55)</f>
-        <v>2.1343603957757012E-4</v>
+        <v>2.077823578085038E-4</v>
       </c>
       <c r="K2">
         <f t="shared" ref="K2:L2" si="0">AVERAGE(H2,H4:H8,H11:H36,H38,H40,H46:H49,H54:H55)</f>
-        <v>2.6105799262448551E-4</v>
+        <v>2.5285981826009176E-4</v>
       </c>
       <c r="L2">
         <f t="shared" si="0"/>
-        <v>4.2684580995438104</v>
-      </c>
-      <c r="M2" s="2">
+        <v>3.7050985420504077</v>
+      </c>
+      <c r="M2" s="1">
         <f>AVERAGE(J2:L2)</f>
-        <v>1.4229775311920043</v>
+        <v>1.2351863947421589</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -531,25 +533,25 @@
         <v>685.50958968000396</v>
       </c>
       <c r="D4">
-        <v>32.1040525815595</v>
+        <v>32.104322440917201</v>
       </c>
       <c r="E4">
-        <v>35.209729165824101</v>
+        <v>35.209955634035097</v>
       </c>
       <c r="F4">
-        <v>685.53439537454301</v>
+        <v>685.68231225709201</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>1.0370295950983703E-4</v>
+        <v>8.7116422287081819E-5</v>
       </c>
       <c r="H4">
         <f t="shared" si="2"/>
-        <v>1.9916407502107091E-5</v>
+        <v>1.8005361522105935E-4</v>
       </c>
       <c r="I4">
         <f t="shared" si="3"/>
-        <v>1.7540274820607517E-2</v>
+        <v>0.12213330552297796</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -563,25 +565,25 @@
         <v>685.51817840597403</v>
       </c>
       <c r="D5">
-        <v>32.104148450861402</v>
+        <v>32.104369868421998</v>
       </c>
       <c r="E5">
-        <v>35.209822715515699</v>
+        <v>35.210004683268401</v>
       </c>
       <c r="F5">
-        <v>685.583927946259</v>
+        <v>685.70617875507003</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>3.2136304165174247E-5</v>
+        <v>1.2442955440581616E-4</v>
       </c>
       <c r="H5">
         <f t="shared" si="2"/>
-        <v>7.4598170887123916E-5</v>
+        <v>2.0326880278027156E-4</v>
       </c>
       <c r="I5">
         <f t="shared" si="3"/>
-        <v>4.6491945795399697E-2</v>
+        <v>0.13293632171122033</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -595,25 +597,25 @@
         <v>706.80045855005596</v>
       </c>
       <c r="D6">
-        <v>32.1035012690594</v>
+        <v>32.103441601101302</v>
       </c>
       <c r="E6">
-        <v>35.209907089240403</v>
+        <v>35.209847443100699</v>
       </c>
       <c r="F6">
-        <v>710.39284148603804</v>
+        <v>708.65735871914501</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>1.1865612334784239E-4</v>
+        <v>1.6084774113847553E-4</v>
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
-        <v>1.3483534076391573E-4</v>
+        <v>1.770115306200537E-4</v>
       </c>
       <c r="I6">
         <f t="shared" si="3"/>
-        <v>2.5401983346517629</v>
+        <v>1.31302670154931</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -627,25 +629,25 @@
         <v>697.83984970695201</v>
       </c>
       <c r="D7">
-        <v>32.103505274424997</v>
+        <v>32.103450393226602</v>
       </c>
       <c r="E7">
-        <v>35.209910588465597</v>
+        <v>35.209855848321602</v>
       </c>
       <c r="F7">
-        <v>710.40028144291398</v>
+        <v>708.830169564681</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>2.8063794660519254E-4</v>
+        <v>3.1944481414972648E-4</v>
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>4.505230677718903E-4</v>
+        <v>4.8923019479355477E-4</v>
       </c>
       <c r="I7">
         <f t="shared" si="3"/>
-        <v>8.8815664551294287</v>
+        <v>7.7713296988093417</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -659,25 +661,25 @@
         <v>703.12334013740201</v>
       </c>
       <c r="D8">
-        <v>32.103726646883402</v>
+        <v>32.103688141940502</v>
       </c>
       <c r="E8">
-        <v>35.2103706815655</v>
+        <v>35.210213999092197</v>
       </c>
       <c r="F8">
-        <v>697.57705092922697</v>
+        <v>701.64272883859701</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>7.7245269247579523E-5</v>
+        <v>5.0018163013845594E-5</v>
       </c>
       <c r="H8">
         <f t="shared" si="2"/>
-        <v>2.1775069755871696E-4</v>
+        <v>1.069594581929094E-4</v>
       </c>
       <c r="I8">
         <f t="shared" si="3"/>
-        <v>3.9218187095223378</v>
+        <v>1.0469502896864382</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -787,25 +789,25 @@
         <v>704.59237322492299</v>
       </c>
       <c r="D12">
-        <v>32.103749574704501</v>
+        <v>32.103816814961</v>
       </c>
       <c r="E12">
-        <v>35.210213679514403</v>
+        <v>35.210350627895899</v>
       </c>
       <c r="F12">
-        <v>710.83821407777702</v>
+        <v>705.99879876967896</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>1.0262597097203173E-4</v>
+        <v>5.5079929633053302E-5</v>
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
-        <v>1.9886823834571027E-4</v>
+        <v>1.0203110911773976E-4</v>
       </c>
       <c r="I12">
         <f t="shared" si="3"/>
-        <v>4.4164764212650542</v>
+        <v>0.99449303993092475</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -819,25 +821,25 @@
         <v>699.98189261949597</v>
       </c>
       <c r="D13">
-        <v>32.103760659619901</v>
+        <v>32.1038773441432</v>
       </c>
       <c r="E13">
-        <v>35.210191536493497</v>
+        <v>35.210483990821501</v>
       </c>
       <c r="F13">
-        <v>699.69307499893205</v>
+        <v>699.76840020417001</v>
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
-        <v>1.4007209700627374E-4</v>
+        <v>5.7563679322232165E-5</v>
       </c>
       <c r="H13">
         <f t="shared" si="2"/>
-        <v>3.3702125059958276E-4</v>
+        <v>1.302248120802389E-4</v>
       </c>
       <c r="I13">
         <f t="shared" si="3"/>
-        <v>0.20422489802690993</v>
+        <v>0.15096193460888041</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -851,25 +853,25 @@
         <v>704.20032558811295</v>
       </c>
       <c r="D14">
-        <v>32.103972061832202</v>
+        <v>32.1038791295626</v>
       </c>
       <c r="E14">
-        <v>35.210678654714002</v>
+        <v>35.210485336548302</v>
       </c>
       <c r="F14">
-        <v>696.42775872243396</v>
+        <v>702.40221241180404</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
-        <v>6.5756762539487037E-5</v>
+        <v>4.3724512583450852E-8</v>
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>1.3139538981006967E-4</v>
+        <v>5.301196082557513E-6</v>
       </c>
       <c r="I14">
         <f t="shared" si="3"/>
-        <v>5.4960347379474772</v>
+        <v>1.271458020308907</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -883,25 +885,25 @@
         <v>702.56833302678297</v>
       </c>
       <c r="D15">
-        <v>32.103781526129701</v>
+        <v>32.103847940305599</v>
       </c>
       <c r="E15">
-        <v>35.210177491052498</v>
+        <v>35.210301260849597</v>
       </c>
       <c r="F15">
-        <v>701.24468174609399</v>
+        <v>700.11639407944404</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
-        <v>7.1280772070728227E-5</v>
+        <v>2.4318857926705453E-5</v>
       </c>
       <c r="H15">
         <f t="shared" si="2"/>
-        <v>1.920074629626977E-4</v>
+        <v>2.7952592579767548E-4</v>
       </c>
       <c r="I15">
         <f t="shared" si="3"/>
-        <v>0.93596279650143432</v>
+        <v>1.7337826567187631</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1107,25 +1109,25 @@
         <v>701.15030442948</v>
       </c>
       <c r="D22">
-        <v>32.104105849500897</v>
+        <v>32.104013506542699</v>
       </c>
       <c r="E22">
-        <v>35.209891078526397</v>
+        <v>35.210131192778398</v>
       </c>
       <c r="F22">
-        <v>699.62184919091601</v>
+        <v>701.18992637829797</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>6.3884247402665981E-5</v>
+        <v>1.4120845335257573E-6</v>
       </c>
       <c r="H22">
         <f t="shared" si="2"/>
-        <v>1.6019703708941314E-4</v>
+        <v>9.5893787603358249E-6</v>
       </c>
       <c r="I22">
         <f t="shared" si="3"/>
-        <v>1.0807810639287014</v>
+        <v>2.8016948693010614E-2</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1139,25 +1141,25 @@
         <v>690.38480141554498</v>
       </c>
       <c r="D23">
-        <v>32.104404087308097</v>
+        <v>32.104151931368598</v>
       </c>
       <c r="E23">
-        <v>35.210577249038998</v>
+        <v>35.2101348427394</v>
       </c>
       <c r="F23">
-        <v>693.55306741376899</v>
+        <v>692.06287521392903</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
-        <v>1.9266204372830585E-4</v>
+        <v>1.4360868991933883E-5</v>
       </c>
       <c r="H23">
         <f t="shared" si="2"/>
-        <v>5.1600176848442755E-4</v>
+        <v>2.0317327399902073E-4</v>
       </c>
       <c r="I23">
         <f t="shared" si="3"/>
-        <v>2.240302371946957</v>
+        <v>1.1865773621688278</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1203,25 +1205,25 @@
         <v>697.70249825517806</v>
       </c>
       <c r="D25">
-        <v>32.103499672173399</v>
+        <v>32.103445993613803</v>
       </c>
       <c r="E25">
-        <v>35.209905694145903</v>
+        <v>35.209851986852399</v>
       </c>
       <c r="F25">
-        <v>710.38987527418601</v>
+        <v>708.81814729650603</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
-        <v>2.8393695611686563E-4</v>
+        <v>3.2189342961115754E-4</v>
       </c>
       <c r="H25">
         <f t="shared" si="2"/>
-        <v>5.0512169194258979E-4</v>
+        <v>5.4309848337786475E-4</v>
       </c>
       <c r="I25">
         <f t="shared" si="3"/>
-        <v>8.9713303256108894</v>
+        <v>7.8599508144127537</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1363,25 +1365,25 @@
         <v>685.54045786497204</v>
       </c>
       <c r="D30">
-        <v>32.104216620730298</v>
+        <v>32.104398438578301</v>
       </c>
       <c r="E30">
-        <v>35.209889235977201</v>
+        <v>35.210035875108098</v>
       </c>
       <c r="F30">
-        <v>685.61914911565304</v>
+        <v>685.72017705803603</v>
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
-        <v>1.7618267260108484E-5</v>
+        <v>1.1094636600299001E-4</v>
       </c>
       <c r="H30">
         <f t="shared" si="2"/>
-        <v>9.0905898813408817E-5</v>
+        <v>1.9459542265771825E-4</v>
       </c>
       <c r="I30">
         <f t="shared" si="3"/>
-        <v>5.5643116976588469E-2</v>
+        <v>0.12708066012492047</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1395,25 +1397,25 @@
         <v>704.22534223331002</v>
       </c>
       <c r="D31">
-        <v>32.1036638011104</v>
+        <v>32.1037030808533</v>
       </c>
       <c r="E31">
-        <v>35.210111633598302</v>
+        <v>35.210151640710102</v>
       </c>
       <c r="F31">
-        <v>710.68688478075296</v>
+        <v>710.75612020005599</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
-        <v>1.5861073077577738E-4</v>
+        <v>1.3083575820786812E-4</v>
       </c>
       <c r="H31">
         <f t="shared" si="2"/>
-        <v>2.7597931513702713E-4</v>
+        <v>2.4769001508797482E-4</v>
       </c>
       <c r="I31">
         <f t="shared" si="3"/>
-        <v>4.5690005522223061</v>
+        <v>4.6179573867097705</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1427,25 +1429,25 @@
         <v>703.43702600691097</v>
       </c>
       <c r="D32">
-        <v>32.103747228638902</v>
+        <v>32.103755987203598</v>
       </c>
       <c r="E32">
-        <v>35.210211917765797</v>
+        <v>35.2102095867671</v>
       </c>
       <c r="F32">
-        <v>710.83408494672994</v>
+        <v>707.58512064495596</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
-        <v>1.0296614491305123E-4</v>
+        <v>9.6772904422609858E-5</v>
       </c>
       <c r="H32">
         <f t="shared" si="2"/>
-        <v>2.2324475687541951E-4</v>
+        <v>2.2489302186112919E-4</v>
       </c>
       <c r="I32">
         <f t="shared" si="3"/>
-        <v>5.230510537182572</v>
+        <v>2.9331458475651733</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1459,25 +1461,25 @@
         <v>692.44518522082205</v>
       </c>
       <c r="D33">
-        <v>32.103910466097297</v>
+        <v>32.103877824337197</v>
       </c>
       <c r="E33">
-        <v>35.209751854228401</v>
+        <v>35.209875929642401</v>
       </c>
       <c r="F33">
-        <v>700.30919889272798</v>
+        <v>698.56178521471702</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
-        <v>5.2584129994220077E-5</v>
+        <v>7.5665339910939458E-5</v>
       </c>
       <c r="H33">
         <f t="shared" si="2"/>
-        <v>1.2561872366827819E-4</v>
+        <v>2.133532902861688E-4</v>
       </c>
       <c r="I33">
         <f t="shared" si="3"/>
-        <v>5.5606973947483995</v>
+        <v>4.3250893334887248</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1491,25 +1493,25 @@
         <v>703.34924007885195</v>
       </c>
       <c r="D34">
-        <v>32.1037469304339</v>
+        <v>32.103757018281101</v>
       </c>
       <c r="E34">
-        <v>35.210211693832498</v>
+        <v>35.210209076039497</v>
       </c>
       <c r="F34">
-        <v>710.83356009880299</v>
+        <v>707.11604706014202</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
-        <v>1.1037156957861931E-4</v>
+        <v>1.0323838441512334E-4</v>
       </c>
       <c r="H34">
         <f t="shared" si="2"/>
-        <v>2.2987119120598966E-4</v>
+        <v>2.3172225038876508E-4</v>
       </c>
       <c r="I34">
         <f t="shared" si="3"/>
-        <v>5.2922134386776181</v>
+        <v>2.6635347598910397</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1619,25 +1621,25 @@
         <v>704.35079589996701</v>
       </c>
       <c r="D38">
-        <v>32.103494371506699</v>
+        <v>32.103427823825399</v>
       </c>
       <c r="E38">
-        <v>35.209901063301103</v>
+        <v>35.209834274682002</v>
       </c>
       <c r="F38">
-        <v>710.38002929877996</v>
+        <v>708.38712077723198</v>
       </c>
       <c r="G38">
         <f t="shared" si="1"/>
-        <v>2.5202909835451717E-5</v>
+        <v>7.2259226554757973E-5</v>
       </c>
       <c r="H38">
         <f t="shared" si="2"/>
-        <v>2.0537711758794133E-4</v>
+        <v>2.526038030603668E-4</v>
       </c>
       <c r="I38">
         <f t="shared" si="3"/>
-        <v>4.2633118216570516</v>
+        <v>2.8541126917860224</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -1683,25 +1685,25 @@
         <v>698.40909309836798</v>
       </c>
       <c r="D40">
-        <v>32.103663934523198</v>
+        <v>32.103709816298903</v>
       </c>
       <c r="E40">
-        <v>35.210111878008703</v>
+        <v>35.210158573971199</v>
       </c>
       <c r="F40">
-        <v>710.68712099198297</v>
+        <v>710.76799296876197</v>
       </c>
       <c r="G40">
         <f t="shared" si="1"/>
-        <v>5.2777172761529325E-5</v>
+        <v>2.0333858027664784E-5</v>
       </c>
       <c r="H40">
         <f t="shared" si="2"/>
-        <v>3.0099470626272307E-4</v>
+        <v>2.6797567452787745E-4</v>
       </c>
       <c r="I40">
         <f t="shared" si="3"/>
-        <v>8.6818767831727417</v>
+        <v>8.7390619063611386</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>